<commit_message>
fixed issue with alignment
</commit_message>
<xml_diff>
--- a/Results/comparison_results/Easy_comparison/ReAct_Easy_langsmith_extraction.xlsx
+++ b/Results/comparison_results/Easy_comparison/ReAct_Easy_langsmith_extraction.xlsx
@@ -458,180 +458,180 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Move Robot6 to location (5, 4) and remove the liquid spill.</t>
+          <t>Move Robot32 to location (2, 9) and remove the toolkit.</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>70.214196</v>
+        <v>66.63938</v>
       </c>
       <c r="C2" t="n">
-        <v>10328</v>
+        <v>9970</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.03054</t>
+          <t>0.02688</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Move Robot29 to location (5, 12) and remove the large debris.</t>
+          <t>Move Robot6 to location (5, 4) and remove the liquid spill.</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72.310749</v>
+        <v>70.214196</v>
       </c>
       <c r="C3" t="n">
-        <v>10285</v>
+        <v>10328</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.02937</t>
+          <t>0.03054</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Move Robot48 to location (6, 6) and remove the dust.</t>
+          <t>Move Robot29 to location (5, 12) and remove the large debris.</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>78.849836</v>
+        <v>72.310749</v>
       </c>
       <c r="C4" t="n">
-        <v>10822</v>
+        <v>10285</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.03405</t>
+          <t>0.02937</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Move Robot41 to location (1, 8) and remove the grass.</t>
+          <t>Move Robot48 to location (6, 6) and remove the dust.</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>78.289986</v>
+        <v>78.849836</v>
       </c>
       <c r="C5" t="n">
-        <v>11156</v>
+        <v>10822</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.03528</t>
+          <t>0.03405</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Move Robot10 to location (9, 5) and remove the small debris.</t>
+          <t>Move Robot41 to location (1, 8) and remove the grass.</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>64.416303</v>
+        <v>78.289986</v>
       </c>
       <c r="C6" t="n">
-        <v>10286</v>
+        <v>11156</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.02802</t>
+          <t>0.03528</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Move Robot13 to location (10, 10) and remove the vehicle.</t>
+          <t>Move Robot10 to location (9, 5) and remove the small debris.</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>67.37535</v>
+        <v>64.416303</v>
       </c>
       <c r="C7" t="n">
-        <v>10614</v>
+        <v>10286</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.03288</t>
+          <t>0.02802</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Move Robot23 to location (8, 2) and remove the construction materials.</t>
+          <t>Move Robot13 to location (10, 10) and remove the vehicle.</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>63.545454</v>
+        <v>67.37535</v>
       </c>
       <c r="C8" t="n">
-        <v>10671</v>
+        <v>10614</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.03114</t>
+          <t>0.03288</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Move Robot24 to location (11, 8) and remove the tree branches.</t>
+          <t>Move Robot23 to location (8, 2) and remove the construction materials.</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>64.912352</v>
+        <v>63.545454</v>
       </c>
       <c r="C9" t="n">
-        <v>10309</v>
+        <v>10671</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.03084</t>
+          <t>0.03114</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Move Robot15 to location (3, 8) and remove the screws.</t>
+          <t>Move Robot24 to location (11, 8) and remove the tree branches.</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>65.80332799999999</v>
+        <v>64.912352</v>
       </c>
       <c r="C10" t="n">
-        <v>10319</v>
+        <v>10309</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.03039</t>
+          <t>0.03084</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Move to location (9, 5) and remove the toolkit.</t>
+          <t>Move Robot15 to location (3, 8) and remove the screws.</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>75.906284</v>
+        <v>65.80332799999999</v>
       </c>
       <c r="C11" t="n">
-        <v>10794</v>
+        <v>10319</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.03354</t>
+          <t>0.03039</t>
         </is>
       </c>
     </row>

</xml_diff>